<commit_message>
Persistencia dos dados de clientes
</commit_message>
<xml_diff>
--- a/Planejamento - SAAS - Stock Manager.xlsx
+++ b/Planejamento - SAAS - Stock Manager.xlsx
@@ -849,7 +849,7 @@
   <dimension ref="B3:X15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="T11" sqref="T11:X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,19 +1265,19 @@
         <v>16</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="W10" s="19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="X10" s="19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:24" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>15</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="U11" s="19" t="s">
         <v>7</v>
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:24" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1359,19 +1359,19 @@
         <v>15</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="U12" s="19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="V12" s="19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="W12" s="19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:24" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1384,7 @@
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="T4:X4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A16:XFD1048576 A14:S15 Y14:XFD15 A1:XFD13">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>

</xml_diff>